<commit_message>
feat: add frumento beers
</commit_message>
<xml_diff>
--- a/scripts/beerz.xlsx
+++ b/scripts/beerz.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivierodotti/repos/beer-champz/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivierodotti/repos/beer-champz/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EA9160-3135-594D-A65E-C2649D36772E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF74ADE-E3C7-9D44-B8CD-99BA1AEB5016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{C104FC75-D894-EC4A-A495-9D083AFB55FF}"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{C104FC75-D894-EC4A-A495-9D083AFB55FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
+    <sheet name="Birre di frumento" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="207">
   <si>
     <t>name</t>
   </si>
@@ -104,9 +105,6 @@
     <t>Birra anglosassone di color ambrato, caratterizzata dallo spiccato aroma fruttato e resinoso tipico dei luppoli nordamericani impiegati sia nelle differenti fasi della cottura che in sede di dry-hopping. L’elevato livello di amaro, bilanciato dal corpo leggermente maltato, non ne pregiudica una certa freschezza al palato.</t>
   </si>
   <si>
-    <t>cippa l'ipa</t>
-  </si>
-  <si>
     <t>Colore dorato intenso e schiuma chiara e persistente. Caratterizzato dai luppoli abbondanti ed aromatici. Prevalgono le note agrumate, miste a sfumature resinose e balsamiche.</t>
   </si>
   <si>
@@ -176,9 +174,6 @@
     <t>birrificio lambrate</t>
   </si>
   <si>
-    <t>Si caratterizza per l'utilizzo massiccio di luppoli americani soprattutto in dry-hopping, i quali le conferiscono esuberanti e freschi profumi agrumati tipici di questo stile americano.</t>
-  </si>
-  <si>
     <t>larkin street</t>
   </si>
   <si>
@@ -276,12 +271,6 @@
   </si>
   <si>
     <t>7.2%</t>
-  </si>
-  <si>
-    <t>E' una american ipa in versione session (cioè con gradazione &lt;= 4.5%). E' di colore biondo chiaro, dagli intensi profumi erbacei e di luppolo dovuti al dry hopping fatto con luppoli americani e neozelandesi, ma anche di cereali e frutta</t>
-  </si>
-  <si>
-    <t>Birra accattivante,  gusto deciso, pieno e con una bella bilanciatura fra la parte maltata e quella luppolata. E' una ipa in pieno stile inglese, con la giusta importanza data al malto e all'amaro finale.</t>
   </si>
   <si>
     <t>Tutta la carica aromatica di una IPA poggiata su un letto di malti scuri. Ha un ampio spettro di profumi che vanno dalla menta alla resina di pino, dal cacao tostato alla buccia di agrumi. Amara e piccante ma anche ben bilanciata. Mai giudicare solamente con gli occhi.</t>
@@ -291,15 +280,9 @@
 Il suo carattere forte deriva da una miscela di luppoli selezionati, che vi accompagneranno in un viaggio sensoriale ineguagliabile.</t>
   </si>
   <si>
-    <t>Birra dal colore ambrato carico. Nell'ampio bouquet aromatico primeggia l'agrumato (pompelmo, mandarino e scorza d'arancia) affiancato da note erbacee, speziate e balsamiche. Durante la beva, note fruttate di pesca e albicocca vengono bilanciate da un'importante luppolatura. Il finale secco e il corpo bilanciato le donano una grande bevibilità.</t>
-  </si>
-  <si>
     <t>San Diego è una birra che incarna lo stile californiano delle West Coast Ipa, dal colore giallo dorato, che gioca sopratutto sull’esplosività dei luppoli e sul magistrale equilibrio gustativo, all’insegna della beverinità. Si fa subito notare per il suo bouquet fruttato di agrumi, frutta esotica e un leggero resinoso, la parte maltata è presente ma preferisce dare la scena ai veri protagonisti di questo spettacolo, i luppoli Made In Usa. La freschezza esotica e il finale secco piacevolmente aromatico rendono la bevuta leggera, celando l’importante gradazione alcolica (7,2%). La San Diego è la scelta perfetta per chi ama lo stile ed è anche Gluten Free.</t>
   </si>
   <si>
-    <t>E' una fantastica american pale ale dal bel colore ambrato. Profumi tipici di agrumi e note erbacee esplodono in bocca con un amaro intenso ma non eccessivo perchè mediato da note caramellate date dai malti.</t>
-  </si>
-  <si>
     <t>IPA</t>
   </si>
   <si>
@@ -315,20 +298,396 @@
     <t>neipa</t>
   </si>
   <si>
-    <t>6.2%%</t>
-  </si>
-  <si>
     <t>La Impavida Tropic Thunder è una DDH Neipa, una India Pale Ale dal profilo spiccatamente tropicale. Dal colore biondo intenso, viene prodotta con un mix di malti inglesi, e una base di avena che creano uno sfondo morbido e vellutato per ospitare le più espressive varietà di luppoli americani e australiani. Profilo estremamente citrico, spiccano i profumi e sapori di frutta tropicale, albicocca e pompelmo per una esplosione amara e fresca.</t>
   </si>
   <si>
     <t>tropic thunder</t>
+  </si>
+  <si>
+    <t>shop</t>
+  </si>
+  <si>
+    <t>https://shop.canediguerra.com/collections/beer/products/berliner-weisse</t>
+  </si>
+  <si>
+    <t>Berliner Weisse</t>
+  </si>
+  <si>
+    <t>Birra acida di frumento dalla tradizione secolare, la specialità berlinese ha negli anni rischiato di scomparire, per poi tornare in voga grazie al recente movimento della birra artigianale. Color giallo paglierino, acidità moderata, corpo elegante e leggero, la versione da noi proposta presenta un caratteristico sapore di cereali e spezie.</t>
+  </si>
+  <si>
+    <t>berliner weiss</t>
+  </si>
+  <si>
+    <t>Bianca</t>
+  </si>
+  <si>
+    <t>blanche</t>
+  </si>
+  <si>
+    <t>Birra chiara, pallida e opalescente, prodotta con un’abbondante percentuale di frumento. Ha una fresca acidità sottolineata da una delicata speziatura, che ne bilanciano la morbidezza tattile.</t>
+  </si>
+  <si>
+    <t>Brùton - San Cassiano di Moriano (LU)</t>
+  </si>
+  <si>
+    <t>https://www.bruton.it/shop/tipologia/blanche/bianca-33/</t>
+  </si>
+  <si>
+    <t>White side</t>
+  </si>
+  <si>
+    <t>https://www.birramiata.com/prodotto/white-side-bott/</t>
+  </si>
+  <si>
+    <t>Birra dal colore giallo torbido e una schiuma bianca morbida e persistente.  Assai gradevole al naso per la lunga scia speziata di coriandolo e buccia d’arancia amara che ben si amalgamano ai luppoli Perle e Styrian.</t>
+  </si>
+  <si>
+    <t>Birra Amiata - Castel del Piano (GR)</t>
+  </si>
+  <si>
+    <t>WEISSBIER</t>
+  </si>
+  <si>
+    <t>weiss</t>
+  </si>
+  <si>
+    <t>Chiamala Weiss, Weizen o birra di frumento, aggiungici un lievito tipico Bavarese e del luppolo Nobile ed il risultato è LA birra estiva per eccellenza! Gli aromi fruttati di banana e i suoi fenoli speziati ti conquisteranno sin dal primo sorso…Ein Prosit!</t>
+  </si>
+  <si>
+    <t>Impavida - Arco (TN)</t>
+  </si>
+  <si>
+    <t>https://www.birraimpavida.com/shop-birre/</t>
+  </si>
+  <si>
+    <t>Bianca piperita</t>
+  </si>
+  <si>
+    <t>Birra d’ispirazione belga, in stile blanche, da cui il nome. Nel rispetto dello stile si impiegano frumento non maltato, avena, buccia d’arancia e coriandolo. E’ caratterizzata dall’utilizzo della menta piperita e del miele di produzione locale.</t>
+  </si>
+  <si>
+    <t>Opperbacco - Notaresco (TE)</t>
+  </si>
+  <si>
+    <t>https://www.cantinadellabirra.it/shop/birra-opperbacco-bianca-piperita.html</t>
+  </si>
+  <si>
+    <t>Cubulteria</t>
+  </si>
+  <si>
+    <t>https://birrakarma.com/classic/cubulteria/</t>
+  </si>
+  <si>
+    <t>Birra chiara doppio malto ad alta fermentazione, prodotta con una miscela di malto di frumento e d’orzo, con particolarità aromatiche dovute all’aggiunta di cannella e bucce d’arancia. È una birra complessa ma nello stesso è elegante e intrigante. Rifermentata e affinata in bottiglia, forma sedimento naturale.</t>
+  </si>
+  <si>
+    <t>italian wheat</t>
+  </si>
+  <si>
+    <t>Karma - Alife (CE)</t>
+  </si>
+  <si>
+    <t>Blanche. Alta fermentazione. L’aggiunta dei fiori di canapa e bucce di agrumi conferisce un sapore piacevolmente acidulo e aromatico, che sconfina nell’erbaceo.</t>
+  </si>
+  <si>
+    <t>spirito agricolo - Fabriano (AN)</t>
+  </si>
+  <si>
+    <t>https://birraecucina.it/le-nostre-birre/</t>
+  </si>
+  <si>
+    <t>Edvige</t>
+  </si>
+  <si>
+    <t>Golden Ale. Alta fermentazione. Birra fresca e agrumata, dai profumi intensi e delicati con uno spiccato sentore vinoso dato dall’utilizzo del Nelson Sauvin. In bocca ha un gusto piacevole e dissetante con una leggera nota amara.</t>
+  </si>
+  <si>
+    <t>Blanche</t>
+  </si>
+  <si>
+    <t>Birrficio Picara - Salemi (TP)</t>
+  </si>
+  <si>
+    <t>https://www.birrificiopicara.it/</t>
+  </si>
+  <si>
+    <t>Lunare</t>
+  </si>
+  <si>
+    <t>Blanche legata al territorio prodotta con grano antico coltivato a Saracena, varietà “Rossetta” e scorze di Piretto di Civita.</t>
+  </si>
+  <si>
+    <t>De Alchemia - Saracena (CS)</t>
+  </si>
+  <si>
+    <t>https://www.dealchemia.it/birre-de-alchemia/</t>
+  </si>
+  <si>
+    <t>birra ofelia - Sovizzo (VI)</t>
+  </si>
+  <si>
+    <t>La Speltina</t>
+  </si>
+  <si>
+    <t>https://www.birraofelia.it/product-page/la-speltina-blanche</t>
+  </si>
+  <si>
+    <t>Waldweg</t>
+  </si>
+  <si>
+    <t>hefe-weizen</t>
+  </si>
+  <si>
+    <t>Birra di frumento leggera e rinfrescante, grazie ad una buona percentuale di frumento, che conferisce la tipica sfumata acidità ed una piacevole sensazione di pulizia al palato, contraddistinta da un corpo snello e dalla grande facilità di beva. Il ceppo di lievito per le Weizen , imprescindibile per questo stile, conferisce le classiche note di banana, pera e chiodi di garofano che si completano con l’utilizzo  molto basso di luppolo, per una birra per nulla amara, adatta soprattutto alle calde giornate estive.</t>
+  </si>
+  <si>
+    <t>https://birrificiofogliederba.it/prodotto/waldweg/</t>
+  </si>
+  <si>
+    <t>Gosexy</t>
+  </si>
+  <si>
+    <t>gose</t>
+  </si>
+  <si>
+    <t>Gose è un vecchio stile di birra acida nato nella città tedesca Goslar.</t>
+  </si>
+  <si>
+    <t>https://batzenshop.com/it/go-sexy</t>
+  </si>
+  <si>
+    <t>Weisse</t>
+  </si>
+  <si>
+    <t>Questa birra di frumento è piacevolmente rinfrescante, fruttata e dalla schiuma fine; ha un gusto intenso di banana e chiodi di garofano con un finale leggermente dolce.</t>
+  </si>
+  <si>
+    <t>https://batzenshop.com/it/weisse</t>
+  </si>
+  <si>
+    <t>Batzen BRÄU - Bolzano</t>
+  </si>
+  <si>
+    <t>Goslar 1826</t>
+  </si>
+  <si>
+    <t>Interpretazione Made in Italy di uno stile tradizionale tedesco, nasce dalla collaborazione con il birrificio La Buttiga di Piacenza. Birra di frumento con utilizzo di batteri lattici selezionati e sale, a naso le note acide e agrumate accompagnano una bevuta dalla bollicina vivace, rinfrescante, piacevolmente acida e sapida.</t>
+  </si>
+  <si>
+    <t>piccolo birrificio clandestino - Livorno</t>
+  </si>
+  <si>
+    <t>https://www.piccolobirrificioclandestino.it/prodotto/goslar-1826/</t>
+  </si>
+  <si>
+    <t>Litha</t>
+  </si>
+  <si>
+    <t>Aspetto velato e colore giallo paglierino. Brassata con l’utilizzo di malto e frumento marchigiani. Le caratteristiche note speziate date dal coriandolo e dal cardamomo la rendono molto fresca e dissetante.</t>
+  </si>
+  <si>
+    <t>mastio - Colmurano (MC)</t>
+  </si>
+  <si>
+    <t>https://www.birrificioilmastio.com/birre/litha/</t>
+  </si>
+  <si>
+    <t>Dunkelweizen</t>
+  </si>
+  <si>
+    <t>Dunkel-weiss</t>
+  </si>
+  <si>
+    <t>birrificio della granda - Lagnasco (CN)</t>
+  </si>
+  <si>
+    <t>https://www.birrificiodellagranda.it/collections/birre-artigianali/products/dunkelweizen-limited-edition?variant=47641294733635</t>
+  </si>
+  <si>
+    <t>Baby Blue</t>
+  </si>
+  <si>
+    <t>saison</t>
+  </si>
+  <si>
+    <t>Collerosso - Borgorose(RI)</t>
+  </si>
+  <si>
+    <t>https://www.cantinadellabirra.it/shop/collerosso-baby-blue.html</t>
+  </si>
+  <si>
+    <t>Jungle Juice - Roma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jellyfish </t>
+  </si>
+  <si>
+    <t>Saison classica con impiego di segale e frumento, al naso esprime una varietà di aromi che spaziano da sentori pepati a fiori bianchi, con sfumature tipiche di frutta gialla, note erbacee, e una manciata di agrumi (limone, cedro).</t>
+  </si>
+  <si>
+    <t>https://www.junglejuicebrewing.com/shopbirre</t>
+  </si>
+  <si>
+    <t>Salty la faina</t>
+  </si>
+  <si>
+    <t>Fiore a tre petali</t>
+  </si>
+  <si>
+    <t>https://www.birrificiosabino.com/shop/fiore-a-tre-petali-bottiglia</t>
+  </si>
+  <si>
+    <t>Birrificio Sabino - Poggio Mirteto (RI)</t>
+  </si>
+  <si>
+    <t>Iggy</t>
+  </si>
+  <si>
+    <t>https://www.birradelleremo.it/birre/iggy-farmhouse/</t>
+  </si>
+  <si>
+    <t>Edina A.</t>
+  </si>
+  <si>
+    <t>saision</t>
+  </si>
+  <si>
+    <t>https://rubiubirra.it/prodotto/edina-a/</t>
+  </si>
+  <si>
+    <r>
+      <t>Una </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Saison classica ma non troppo, secca al palato ma pepata e agrumata insieme. Nove luppoli in ricetta la rendono fresca e moderna così come fu Edina Altara, poliedrica artista sarda a cui si ispira. Segui la strada del cuore, prendi la scelta azzardata che vince la sfida e rivela la tua vera natura.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>La </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF3A3A3A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Blanche Picara è una birra artigianale Siciliana fresca e beverina, dall’aroma speziato e dal sapore agrumato. Prodotta con malto d’orzo e grano Capeiti. I suoi aromi agrumati provengono dal coriandolo e dalla buccia d’arancia</t>
+    </r>
+  </si>
+  <si>
+    <t>Canediguerra - Alessandria</t>
+  </si>
+  <si>
+    <t>Blanche realizzata con il farro Spelta coltivato a Sovizzo (VI). La buccia di limone, i fiori di sambuco e il pepe utilizzati rendono questa birra fresca, piacevole e beverina.</t>
+  </si>
+  <si>
+    <t>3.2%</t>
+  </si>
+  <si>
+    <t>5.3%</t>
+  </si>
+  <si>
+    <t>5.2%</t>
+  </si>
+  <si>
+    <t>4.6%</t>
+  </si>
+  <si>
+    <t>6.5%</t>
+  </si>
+  <si>
+    <t>5.6%</t>
+  </si>
+  <si>
+    <t>5.0%</t>
+  </si>
+  <si>
+    <t>5.5%</t>
+  </si>
+  <si>
+    <t>5.1%</t>
+  </si>
+  <si>
+    <t>4.3%</t>
+  </si>
+  <si>
+    <t>4.9%</t>
+  </si>
+  <si>
+    <t>6.0%</t>
+  </si>
+  <si>
+    <t>4.7%</t>
+  </si>
+  <si>
+    <t>6.4%</t>
+  </si>
+  <si>
+    <t>8.0%</t>
+  </si>
+  <si>
+    <t>7.0%</t>
+  </si>
+  <si>
+    <t>E’ una fantastica american pale ale dal bel colore ambrato. Profumi tipici di agrumi e note erbacee esplodono in bocca con un amaro intenso ma non eccessivo perchè mediato da note caramellate date dai malti.</t>
+  </si>
+  <si>
+    <t>E’ una american ipa in versione session (cioè con gradazione &lt;= 4.5%). E’ di colore biondo chiaro, dagli intensi profumi erbacei e di luppolo dovuti al dry hopping fatto con luppoli americani e neozelandesi, ma anche di cereali e frutta</t>
+  </si>
+  <si>
+    <t>cippa l’ipa</t>
+  </si>
+  <si>
+    <t>Birra accattivante,  gusto deciso, pieno e con una bella bilanciatura fra la parte maltata e quella luppolata. E’ una ipa in pieno stile inglese, con la giusta importanza data al malto e all’amaro finale.</t>
+  </si>
+  <si>
+    <t>Si caratterizza per l’utilizzo massiccio di luppoli americani soprattutto in dry-hopping, i quali le conferiscono esuberanti e freschi profumi agrumati tipici di questo stile americano.</t>
+  </si>
+  <si>
+    <t>Birra dal colore ambrato carico. Nell’ampio bouquet aromatico primeggia l’agrumato (pompelmo, mandarino e scorza d’arancia) affiancato da note erbacee, speziate e balsamiche. Durante la beva, note fruttate di pesca e albicocca vengono bilanciate da un’importante luppolatura. Il finale secco e il corpo bilanciato le donano una grande bevibilità.</t>
+  </si>
+  <si>
+    <t>St’orta</t>
+  </si>
+  <si>
+    <t>Foglie d’erba - Forni di sopra (UD)</t>
+  </si>
+  <si>
+    <t>Una versione più intensa della classica birra di grano tedesca. Con il tradizionale lievito Weizen che sprigiona l’aroma di banana e l’aggiunta di malti scuri, questa birra regala un caratteristico colore ambrato e una complessità gustativa unica.</t>
+  </si>
+  <si>
+    <t>Una Saison ispirata al classico stile belga ma in chiave contemporanea. Dal colore ambrato con riflessi rosati Baby Blue viene realizzata con aggiunta di una miscela innovativa a base di ibisco, scorza d’arancia e ginepro. Al naso i sentori sono intensi con in evidenza note di lievito, luppolo e spezie</t>
+  </si>
+  <si>
+    <t>Una birra ispirata alle produzioni tradizionali della zona di Lipsia condita con il lievito della nostra Ute. Un prodotto dall’equilibrio estremo e da una delicata sfumatura salina.</t>
+  </si>
+  <si>
+    <t>Saison in stile belga realizzata con farro, segnale e frumento. Dal colore dorato è intensamente aromatica e profumata; al naso percepiamo avvolgenti note di camomilla, fieno, frutta a pasta gialla e fiori di campo. Rustica e fresca al palato, anche qui ritroviamo i sentori dell’aroma, bevuta esile e scorrevole. Finale secco e pulito.</t>
+  </si>
+  <si>
+    <t>Rustica, complessa ed elegante Iggy fa parte della serie Bootleg di Birra dell’Eremo ed è una Farmhouse Ale a fermentazione spontanea, invecchiata in botte e realizzata con luppolo Surannè ed aggiunta di segale e frumento. Versata nel bicchiere si svela di un invitante colore dorato velato; al naso l’aroma è pungente con in evidenza note agrumate di limone, sentori fruttati e sfumature di cantina. Al palato si percepisce una vivace acidità, con lievi sentori lignei dati dal passaggio in botte e decise note funky. Acida ed elegante nel finale.</t>
+  </si>
+  <si>
+    <t>Birra dell’eremo - Assisi (PG)</t>
+  </si>
+  <si>
+    <t>Rubiu - Sant’Antioco (SU)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -346,6 +705,26 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri (Corpo)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3A3A3A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -365,10 +744,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -377,8 +757,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -693,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A9AAD2A-A17E-6A44-94D7-C959B8707D50}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -724,19 +1106,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -746,8 +1128,8 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1">
-        <v>0.08</v>
+      <c r="C3" s="1" t="s">
+        <v>190</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -763,11 +1145,11 @@
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1">
-        <v>0.05</v>
+      <c r="C4" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="D4" t="s">
-        <v>86</v>
+        <v>192</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -781,10 +1163,10 @@
         <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>80</v>
+        <v>193</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -797,11 +1179,11 @@
       <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1">
-        <v>0.06</v>
+      <c r="C6" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
@@ -815,7 +1197,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
@@ -826,321 +1208,826 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>194</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1">
-        <v>7.0000000000000007E-2</v>
+      <c r="C8" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
         <v>23</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
         <v>26</v>
       </c>
-      <c r="E9" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="C10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" t="s">
+        <v>195</v>
+      </c>
+      <c r="E10" t="s">
         <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>32</v>
-      </c>
-      <c r="E11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="1">
-        <v>0.05</v>
+      <c r="C12" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
         <v>36</v>
-      </c>
-      <c r="E12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="1">
-        <v>7.0000000000000007E-2</v>
+      <c r="C13" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
         <v>40</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>42</v>
-      </c>
-      <c r="E14" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="2">
-        <v>0.06</v>
+      <c r="C15" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>196</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="2">
-        <v>0.08</v>
+      <c r="C16" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="2">
-        <v>7.0000000000000007E-2</v>
+      <c r="C17" s="2" t="s">
+        <v>191</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="2">
-        <v>0.08</v>
+      <c r="C20" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="D20" t="s">
-        <v>84</v>
+        <v>197</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" t="s">
         <v>60</v>
-      </c>
-      <c r="B21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" t="s">
-        <v>63</v>
-      </c>
-      <c r="E21" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="2">
-        <v>0.08</v>
+      <c r="C22" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="D22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
         <v>65</v>
       </c>
-      <c r="E22" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="C23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" t="s">
         <v>66</v>
-      </c>
-      <c r="B23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" t="s">
-        <v>85</v>
-      </c>
-      <c r="E23" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="2">
-        <v>0.06</v>
+        <v>33</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="D24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B25" t="s">
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D25" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E25" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="26" x14ac:dyDescent="0.3">
       <c r="D26" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="26" x14ac:dyDescent="0.3">
       <c r="D28" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DD4537-3DEA-F64A-B543-ECF1FB840187}">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="88.5" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>198</v>
+      </c>
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D10" t="s">
+        <v>173</v>
+      </c>
+      <c r="E10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" t="s">
+        <v>126</v>
+      </c>
+      <c r="F11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" t="s">
+        <v>175</v>
+      </c>
+      <c r="E12" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E13" t="s">
+        <v>199</v>
+      </c>
+      <c r="F13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D14" t="s">
+        <v>137</v>
+      </c>
+      <c r="E14" t="s">
+        <v>142</v>
+      </c>
+      <c r="F14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D15" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" t="s">
+        <v>142</v>
+      </c>
+      <c r="F15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" t="s">
+        <v>144</v>
+      </c>
+      <c r="E16" t="s">
+        <v>145</v>
+      </c>
+      <c r="F16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>147</v>
+      </c>
+      <c r="B17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E17" t="s">
+        <v>149</v>
+      </c>
+      <c r="F17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B18" t="s">
+        <v>152</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D18" t="s">
+        <v>200</v>
+      </c>
+      <c r="E18" t="s">
+        <v>153</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" t="s">
+        <v>201</v>
+      </c>
+      <c r="E19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D20" t="s">
+        <v>161</v>
+      </c>
+      <c r="E20" t="s">
+        <v>159</v>
+      </c>
+      <c r="F20" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>163</v>
+      </c>
+      <c r="B21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D21" t="s">
+        <v>202</v>
+      </c>
+      <c r="E21" t="s">
+        <v>159</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>164</v>
+      </c>
+      <c r="B22" t="s">
+        <v>156</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D22" t="s">
+        <v>203</v>
+      </c>
+      <c r="E22" t="s">
+        <v>166</v>
+      </c>
+      <c r="F22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>167</v>
+      </c>
+      <c r="B23" t="s">
+        <v>156</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D23" t="s">
+        <v>204</v>
+      </c>
+      <c r="E23" t="s">
+        <v>205</v>
+      </c>
+      <c r="F23" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>169</v>
+      </c>
+      <c r="B24" t="s">
+        <v>170</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D24" t="s">
+        <v>172</v>
+      </c>
+      <c r="E24" t="s">
+        <v>206</v>
+      </c>
+      <c r="F24" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F21" r:id="rId1" xr:uid="{660D3BCD-E288-BA44-B3C8-4984944C5176}"/>
+    <hyperlink ref="F18" r:id="rId2" xr:uid="{313DCB0A-21FA-4544-A164-AE6A4B45C8D6}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>